<commit_message>
proctor to student warning added
</commit_message>
<xml_diff>
--- a/public/assets/tempfiles/proctors.xlsx
+++ b/public/assets/tempfiles/proctors.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">instId</t>
   </si>
@@ -40,13 +40,37 @@
     <t xml:space="preserve">subjectList</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pawan.khade@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub_01,Both_01</t>
+    <t xml:space="preserve">proctor1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor1@g.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub_01,Both_01,All_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor2@g.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor3@g.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor4@g.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proctor5@g.com</t>
   </si>
 </sst>
 </file>
@@ -56,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,9 +111,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -124,7 +156,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,8 +180,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,22 +197,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -203,7 +247,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0563C1"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -236,7 +280,7 @@
       <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF212529"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -247,18 +291,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,7 +325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>531</v>
       </c>
@@ -289,7 +333,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>9764465052</v>
+        <v>8971648017</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
@@ -297,13 +341,97 @@
       <c r="E2" s="3" t="n">
         <v>12345678</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>531</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>8971648018</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>531</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>8971648019</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>531</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>8971648020</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>531</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>8971648021</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="pawan.khade@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="proctor1@g.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="proctor2@g.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="proctor3@g.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="proctor4@g.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="proctor5@g.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>